<commit_message>
continuation of work #4
</commit_message>
<xml_diff>
--- a/01_Financial_Analysis/FV_practice.xlsx
+++ b/01_Financial_Analysis/FV_practice.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a44ee3842bd9bdcb/_Tech/_git_repos/dc_fin_reporting_in_powerbi/01_Financial_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{7DFE260A-887E-4385-B316-87B89CF1D382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0E0726D-D8E1-450B-AB61-334AB3B4CF3F}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="8_{7DFE260A-887E-4385-B316-87B89CF1D382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{041D3D08-94B4-4747-AD7E-48837BE345C8}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="2655" windowWidth="21600" windowHeight="11205" xr2:uid="{FC0C4777-6E39-495D-AE5C-2965A991161F}"/>
+    <workbookView xWindow="58815" yWindow="1065" windowWidth="16485" windowHeight="17775" activeTab="1" xr2:uid="{FC0C4777-6E39-495D-AE5C-2965A991161F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Investment</t>
   </si>
@@ -54,16 +55,62 @@
   </si>
   <si>
     <t>Period (yrs)</t>
+  </si>
+  <si>
+    <t>FV</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>yrs</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>comp</t>
+  </si>
+  <si>
+    <t>per year</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Stocks</t>
+  </si>
+  <si>
+    <t>Lump sum</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>Annuities</t>
+  </si>
+  <si>
+    <t>pmt</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>first payment starts today</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,13 +134,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,12 +187,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,6 +227,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF25D146-17DB-490E-9B8D-FA79994BF1E2}">
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -528,4 +630,178 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A91488-E44B-471D-BBE1-98AA7560E1C8}">
+  <dimension ref="B2:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="8">
+        <f>PV(0.02/365,18*365,0,100000)*(-1)</f>
+        <v>69768.320704459256</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="11">
+        <f>PV(0.1/365,18*365,0,100000)*(-1)</f>
+        <v>16533.964443230485</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="4" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E9)</f>
+        <v>=PV(0.1/365,18*365,0,100000)*(-1)</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="4" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(C9)</f>
+        <v>=PV(0.02/365,18*365,0,100000)*(-1)</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="16">
+        <v>428000000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1">
+        <v>30000000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="17">
+        <f>PV(0.075,30,-30000000,0,1)</f>
+        <v>380884957.06502384</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>